<commit_message>
fix: done report access homepage & product
</commit_message>
<xml_diff>
--- a/server/ReportForm.xlsx
+++ b/server/ReportForm.xlsx
@@ -105,14 +105,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,64 +417,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="12.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="4" max="4" width="8.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="49" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" style="2" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="2:4" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:E6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Done: Report access value
</commit_message>
<xml_diff>
--- a/server/ReportForm.xlsx
+++ b/server/ReportForm.xlsx
@@ -22,12 +22,6 @@
     <t>Thời gian:</t>
   </si>
   <si>
-    <t>1. Lượng người dùng truy cập trang chủ:</t>
-  </si>
-  <si>
-    <t>2. Lượng người dùng truy cập trang chi tiết sản phẩm:</t>
-  </si>
-  <si>
     <t>Doanh nghiệp</t>
   </si>
   <si>
@@ -35,6 +29,12 @@
   </si>
   <si>
     <t>Số lượng truy cập</t>
+  </si>
+  <si>
+    <t>2. Lượt truy cập các trang chi tiết sản phẩm:</t>
+  </si>
+  <si>
+    <t>1. Số lượt truy cập trang chủ:</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -449,24 +449,24 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>